<commit_message>
update and improve y2y Fig
</commit_message>
<xml_diff>
--- a/data/sms_vaccination_data.xlsx
+++ b/data/sms_vaccination_data.xlsx
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="B77" zoomScale="116" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1827,6 +1827,221 @@
         <v>72.2</v>
       </c>
     </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>44515</v>
+      </c>
+      <c r="B87" s="1">
+        <v>44502</v>
+      </c>
+      <c r="C87">
+        <v>584.20000000000005</v>
+      </c>
+      <c r="D87">
+        <f>D71</f>
+        <v>284.39999999999998</v>
+      </c>
+      <c r="E87">
+        <v>111.1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="1">
+        <v>44503</v>
+      </c>
+      <c r="C88">
+        <v>686.1</v>
+      </c>
+      <c r="D88">
+        <f t="shared" ref="D88:D102" si="0">D72</f>
+        <v>289.7</v>
+      </c>
+      <c r="E88">
+        <v>119.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B89" s="1">
+        <v>44504</v>
+      </c>
+      <c r="C89">
+        <v>747.2</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="0"/>
+        <v>336.4</v>
+      </c>
+      <c r="E89">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B90" s="1">
+        <v>44505</v>
+      </c>
+      <c r="C90">
+        <v>830.5</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="0"/>
+        <v>385.7</v>
+      </c>
+      <c r="E90">
+        <v>138.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B91" s="1">
+        <v>44506</v>
+      </c>
+      <c r="C91">
+        <v>907.4</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="0"/>
+        <v>415.8</v>
+      </c>
+      <c r="E91">
+        <v>140.6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="1">
+        <v>44507</v>
+      </c>
+      <c r="C92">
+        <v>965.6</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+      <c r="E92">
+        <v>141.80000000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="1">
+        <v>44508</v>
+      </c>
+      <c r="C93">
+        <v>1002.8</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="0"/>
+        <v>491.3</v>
+      </c>
+      <c r="E93">
+        <v>141.1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="1">
+        <v>44509</v>
+      </c>
+      <c r="C94">
+        <v>1076.5999999999999</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="0"/>
+        <v>483.7</v>
+      </c>
+      <c r="E94">
+        <v>143.9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B95" s="1">
+        <v>44510</v>
+      </c>
+      <c r="C95">
+        <v>1188.5999999999999</v>
+      </c>
+      <c r="D95">
+        <f>D79</f>
+        <v>459.4</v>
+      </c>
+      <c r="E95">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B96" s="1">
+        <v>44511</v>
+      </c>
+      <c r="C96">
+        <v>1339.4</v>
+      </c>
+      <c r="D96">
+        <f>D86</f>
+        <v>521.9</v>
+      </c>
+      <c r="E96">
+        <v>110.4</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B97" s="1">
+        <v>44512</v>
+      </c>
+      <c r="C97">
+        <v>1492.8</v>
+      </c>
+      <c r="D97">
+        <v>569</v>
+      </c>
+      <c r="E97">
+        <v>91.4</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B98" s="1">
+        <v>44513</v>
+      </c>
+      <c r="C98">
+        <v>1604</v>
+      </c>
+      <c r="D98">
+        <v>620.70000000000005</v>
+      </c>
+      <c r="E98">
+        <v>77.7</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B99" s="1">
+        <v>44514</v>
+      </c>
+      <c r="C99">
+        <v>1675</v>
+      </c>
+      <c r="D99">
+        <v>670.9</v>
+      </c>
+      <c r="E99">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B100" s="1">
+        <v>44515</v>
+      </c>
+      <c r="C100">
+        <v>1718.3</v>
+      </c>
+      <c r="D100">
+        <v>754.3</v>
+      </c>
+      <c r="E100">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>